<commit_message>
input and results (260131-2032)
</commit_message>
<xml_diff>
--- a/results/RIMP-03_260131-2032/ReqPowDATA.xlsx
+++ b/results/RIMP-03_260131-2032/ReqPowDATA.xlsx
@@ -502,64 +502,64 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>105.2242264198533</v>
+        <v>98.04961276102425</v>
       </c>
       <c r="C2" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="D2" t="n">
-        <v>1350.951632705357</v>
+        <v>1258.85843638851</v>
       </c>
       <c r="E2" t="n">
-        <v>2104.484528397067</v>
+        <v>1960.992255220485</v>
       </c>
       <c r="F2" t="n">
-        <v>2104.484528397067</v>
+        <v>1960.992255220485</v>
       </c>
       <c r="G2" t="n">
-        <v>1895.916816972823</v>
+        <v>1598.469839612929</v>
       </c>
       <c r="H2" t="n">
-        <v>1895.916816972823</v>
+        <v>1598.469839612929</v>
       </c>
       <c r="I2" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="J2" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="K2" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="L2" t="n">
-        <v>2104.484528397067</v>
+        <v>1960.992255220485</v>
       </c>
       <c r="M2" t="n">
-        <v>2104.484528397067</v>
+        <v>1960.992255220485</v>
       </c>
       <c r="N2" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="O2" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="P2" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="Q2" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="R2" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="S2" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="T2" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="U2" t="n">
-        <v>105.2242264198533</v>
+        <v>98.04961276102425</v>
       </c>
     </row>
     <row r="3">
@@ -569,64 +569,64 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>105.2242264198533</v>
+        <v>98.04961276102425</v>
       </c>
       <c r="C3" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="D3" t="n">
-        <v>1078.875429655709</v>
+        <v>1005.334193409084</v>
       </c>
       <c r="E3" t="n">
-        <v>1696.370223822595</v>
+        <v>1580.705890751345</v>
       </c>
       <c r="F3" t="n">
-        <v>1696.370223822595</v>
+        <v>1580.705890751345</v>
       </c>
       <c r="G3" t="n">
-        <v>1963.841983122465</v>
+        <v>1655.735457629397</v>
       </c>
       <c r="H3" t="n">
-        <v>1963.841983122465</v>
+        <v>1655.735457629397</v>
       </c>
       <c r="I3" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="J3" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="K3" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="L3" t="n">
-        <v>1696.370223822595</v>
+        <v>1580.705890751345</v>
       </c>
       <c r="M3" t="n">
-        <v>1696.370223822595</v>
+        <v>1580.705890751345</v>
       </c>
       <c r="N3" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="O3" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="P3" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="Q3" t="n">
-        <v>1772.78958984438</v>
+        <v>1494.6688982533</v>
       </c>
       <c r="R3" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="S3" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="T3" t="n">
-        <v>210.4484528397067</v>
+        <v>196.0992255220485</v>
       </c>
       <c r="U3" t="n">
-        <v>105.2242264198533</v>
+        <v>98.04961276102425</v>
       </c>
     </row>
     <row r="4">
@@ -642,19 +642,19 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>272.0762030496479</v>
+        <v>253.5242429794263</v>
       </c>
       <c r="E4" t="n">
-        <v>408.1143045744719</v>
+        <v>380.2863644691395</v>
       </c>
       <c r="F4" t="n">
-        <v>408.1143045744719</v>
+        <v>380.2863644691395</v>
       </c>
       <c r="G4" t="n">
-        <v>-67.92516614964215</v>
+        <v>-57.26561801646823</v>
       </c>
       <c r="H4" t="n">
-        <v>-67.92516614964215</v>
+        <v>-57.26561801646823</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -666,10 +666,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>408.1143045744719</v>
+        <v>380.2863644691395</v>
       </c>
       <c r="M4" t="n">
-        <v>408.1143045744719</v>
+        <v>380.2863644691395</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>

</xml_diff>